<commit_message>
word and char tf-idf
mengitung similaritas berdasarkan kata dan huruf
</commit_message>
<xml_diff>
--- a/hasil/hasil_scoring.xlsx
+++ b/hasil/hasil_scoring.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\python\essay_scoring\hasil\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FC6C89-7C31-4264-9706-9457E535B18D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="1425" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="123">
   <si>
     <t>cosine_skor</t>
   </si>
@@ -389,16 +383,13 @@
   </si>
   <si>
     <t>yaitu menelfon biro perjalanan dengan no yang sudah dicantumkan kunjungib website biro perjalanan</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,108 +450,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1256D406-2BCD-4605-B6F6-3BDA8A9E7DB3}" name="Table2" displayName="Table2" ref="A1:Q101" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:Q101" xr:uid="{A476ABAA-F8A1-4A33-8227-900B631DD1BB}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{1F24932C-5D02-49D3-8264-AE80873594F8}" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{46692B25-3511-48B2-9C06-4A409E5C5365}" name="cosine_skor"/>
-    <tableColumn id="3" xr3:uid="{DC92E167-09D4-4AB4-A006-C48E81CB843A}" name="cosine_qualifikasi"/>
-    <tableColumn id="4" xr3:uid="{1535F864-C348-46CC-8571-344EB34A8C72}" name="cosine_similarity"/>
-    <tableColumn id="5" xr3:uid="{3304C4DA-981D-4076-A2BF-2B3ED4F72B5A}" name="cosine_status"/>
-    <tableColumn id="6" xr3:uid="{77C6C80D-106B-4166-A2B6-3D92CFA5466B}" name="cosine_cwm"/>
-    <tableColumn id="7" xr3:uid="{5909B2C9-D0F4-4B56-B452-E168CEADC361}" name="dice_skor"/>
-    <tableColumn id="8" xr3:uid="{05EAB60D-9DA2-485D-8EE1-E57F7BFC0E39}" name="dice_qualifikasi"/>
-    <tableColumn id="9" xr3:uid="{1B4EB8BE-4965-467E-BBE0-8A1E578C39B3}" name="dice_similarity"/>
-    <tableColumn id="10" xr3:uid="{2792C76E-4EA1-49E6-88A2-390897C9582E}" name="dice_status"/>
-    <tableColumn id="11" xr3:uid="{17B8EDAF-D570-4254-B146-84A1467AAEB0}" name="dice_cwm"/>
-    <tableColumn id="12" xr3:uid="{EBCC3A54-612D-4803-B30C-83DC2519EE31}" name="jaccard_skor"/>
-    <tableColumn id="13" xr3:uid="{FCD96A30-0FFB-4269-A8EE-5DE603A7E75A}" name="jaccard_qualifikasi"/>
-    <tableColumn id="14" xr3:uid="{16E6898E-1A67-45CA-A930-DB1085323E83}" name="jaccard_similarity"/>
-    <tableColumn id="15" xr3:uid="{A588D2A0-2071-47E3-9C51-B5D4CA9CCF85}" name="jaccard_status"/>
-    <tableColumn id="16" xr3:uid="{18F5855B-5AEE-4349-87D3-00E2D0D07A67}" name="jaccard_cwm"/>
-    <tableColumn id="17" xr3:uid="{3B82DC20-C155-46FB-B145-A8F89490435B}" name="jawaban"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -606,7 +498,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -638,27 +530,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,24 +564,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,38 +739,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>123</v>
-      </c>
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -964,7 +796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1017,7 +849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1028,7 +860,7 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>0.91400000000000003</v>
+        <v>0.914</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -1043,7 +875,7 @@
         <v>17</v>
       </c>
       <c r="I3">
-        <v>0.91400000000000003</v>
+        <v>0.914</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -1058,7 +890,7 @@
         <v>17</v>
       </c>
       <c r="N3">
-        <v>0.84199999999999997</v>
+        <v>0.842</v>
       </c>
       <c r="O3" t="s">
         <v>18</v>
@@ -1070,12 +902,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -1090,7 +922,7 @@
         <v>21</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
@@ -1105,13 +937,13 @@
         <v>21</v>
       </c>
       <c r="L4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
         <v>16</v>
       </c>
       <c r="N4">
-        <v>0.81799999999999995</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="O4" t="s">
         <v>18</v>
@@ -1123,7 +955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1176,7 +1008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1229,7 +1061,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1240,7 +1072,7 @@
         <v>16</v>
       </c>
       <c r="D7">
-        <v>0.99199999999999999</v>
+        <v>0.992</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -1255,7 +1087,7 @@
         <v>16</v>
       </c>
       <c r="I7">
-        <v>0.99199999999999999</v>
+        <v>0.992</v>
       </c>
       <c r="J7" t="s">
         <v>18</v>
@@ -1270,7 +1102,7 @@
         <v>16</v>
       </c>
       <c r="N7">
-        <v>0.98399999999999999</v>
+        <v>0.984</v>
       </c>
       <c r="O7" t="s">
         <v>18</v>
@@ -1282,7 +1114,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1323,7 +1155,7 @@
         <v>16</v>
       </c>
       <c r="N8">
-        <v>0.90500000000000003</v>
+        <v>0.905</v>
       </c>
       <c r="O8" t="s">
         <v>18</v>
@@ -1335,7 +1167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1346,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>0.99199999999999999</v>
+        <v>0.992</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -1361,7 +1193,7 @@
         <v>16</v>
       </c>
       <c r="I9">
-        <v>0.99199999999999999</v>
+        <v>0.992</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
@@ -1376,7 +1208,7 @@
         <v>16</v>
       </c>
       <c r="N9">
-        <v>0.98399999999999999</v>
+        <v>0.984</v>
       </c>
       <c r="O9" t="s">
         <v>18</v>
@@ -1388,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1441,12 +1273,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -1461,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="G11">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -1476,7 +1308,7 @@
         <v>21</v>
       </c>
       <c r="L11">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M11" t="s">
         <v>17</v>
@@ -1494,7 +1326,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1547,7 +1379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1600,7 +1432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1653,7 +1485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1706,7 +1538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1759,7 +1591,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1812,7 +1644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1865,12 +1697,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1918,7 +1750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1926,10 +1758,10 @@
         <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>0.97199999999999998</v>
+        <v>0.972</v>
       </c>
       <c r="E20" t="s">
         <v>18</v>
@@ -1941,10 +1773,10 @@
         <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I20">
-        <v>0.97199999999999998</v>
+        <v>0.972</v>
       </c>
       <c r="J20" t="s">
         <v>18</v>
@@ -1956,10 +1788,10 @@
         <v>70</v>
       </c>
       <c r="M20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N20">
-        <v>0.94499999999999995</v>
+        <v>0.945</v>
       </c>
       <c r="O20" t="s">
         <v>18</v>
@@ -1971,12 +1803,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2024,7 +1856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2035,7 +1867,7 @@
         <v>16</v>
       </c>
       <c r="D22">
-        <v>0.92700000000000005</v>
+        <v>0.927</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
@@ -2050,7 +1882,7 @@
         <v>16</v>
       </c>
       <c r="I22">
-        <v>0.92700000000000005</v>
+        <v>0.927</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>
@@ -2065,7 +1897,7 @@
         <v>16</v>
       </c>
       <c r="N22">
-        <v>0.86299999999999999</v>
+        <v>0.863</v>
       </c>
       <c r="O22" t="s">
         <v>18</v>
@@ -2077,7 +1909,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2130,7 +1962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2141,7 +1973,7 @@
         <v>16</v>
       </c>
       <c r="D24">
-        <v>0.98599999999999999</v>
+        <v>0.986</v>
       </c>
       <c r="E24" t="s">
         <v>18</v>
@@ -2156,7 +1988,7 @@
         <v>16</v>
       </c>
       <c r="I24">
-        <v>0.98599999999999999</v>
+        <v>0.986</v>
       </c>
       <c r="J24" t="s">
         <v>18</v>
@@ -2171,7 +2003,7 @@
         <v>16</v>
       </c>
       <c r="N24">
-        <v>0.97199999999999998</v>
+        <v>0.972</v>
       </c>
       <c r="O24" t="s">
         <v>18</v>
@@ -2183,7 +2015,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2224,7 +2056,7 @@
         <v>17</v>
       </c>
       <c r="N25">
-        <v>0.77500000000000002</v>
+        <v>0.775</v>
       </c>
       <c r="O25" t="s">
         <v>19</v>
@@ -2236,7 +2068,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2247,7 +2079,7 @@
         <v>16</v>
       </c>
       <c r="D26">
-        <v>0.52400000000000002</v>
+        <v>0.524</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -2262,7 +2094,7 @@
         <v>16</v>
       </c>
       <c r="I26">
-        <v>0.52400000000000002</v>
+        <v>0.524</v>
       </c>
       <c r="J26" t="s">
         <v>19</v>
@@ -2277,7 +2109,7 @@
         <v>16</v>
       </c>
       <c r="N26">
-        <v>0.35499999999999998</v>
+        <v>0.355</v>
       </c>
       <c r="O26" t="s">
         <v>20</v>
@@ -2289,7 +2121,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2300,7 +2132,7 @@
         <v>17</v>
       </c>
       <c r="D27">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -2315,7 +2147,7 @@
         <v>17</v>
       </c>
       <c r="I27">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J27" t="s">
         <v>19</v>
@@ -2330,7 +2162,7 @@
         <v>17</v>
       </c>
       <c r="N27">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O27" t="s">
         <v>20</v>
@@ -2342,18 +2174,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
@@ -2362,13 +2194,13 @@
         <v>21</v>
       </c>
       <c r="G28">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H28" t="s">
         <v>17</v>
       </c>
       <c r="I28">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J28" t="s">
         <v>19</v>
@@ -2377,13 +2209,13 @@
         <v>21</v>
       </c>
       <c r="L28">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M28" t="s">
         <v>17</v>
       </c>
       <c r="N28">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O28" t="s">
         <v>20</v>
@@ -2395,7 +2227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2436,7 +2268,7 @@
         <v>17</v>
       </c>
       <c r="N29">
-        <v>0.33500000000000002</v>
+        <v>0.335</v>
       </c>
       <c r="O29" t="s">
         <v>20</v>
@@ -2448,18 +2280,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30">
-        <v>0.84199999999999997</v>
+        <v>0.842</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
@@ -2468,13 +2300,13 @@
         <v>21</v>
       </c>
       <c r="G30">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H30" t="s">
         <v>16</v>
       </c>
       <c r="I30">
-        <v>0.84199999999999997</v>
+        <v>0.842</v>
       </c>
       <c r="J30" t="s">
         <v>18</v>
@@ -2483,13 +2315,13 @@
         <v>21</v>
       </c>
       <c r="L30">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M30" t="s">
         <v>16</v>
       </c>
       <c r="N30">
-        <v>0.72799999999999998</v>
+        <v>0.728</v>
       </c>
       <c r="O30" t="s">
         <v>19</v>
@@ -2501,7 +2333,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2512,7 +2344,7 @@
         <v>17</v>
       </c>
       <c r="D31">
-        <v>0.70899999999999996</v>
+        <v>0.709</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
@@ -2527,7 +2359,7 @@
         <v>17</v>
       </c>
       <c r="I31">
-        <v>0.70899999999999996</v>
+        <v>0.709</v>
       </c>
       <c r="J31" t="s">
         <v>19</v>
@@ -2542,7 +2374,7 @@
         <v>17</v>
       </c>
       <c r="N31">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="O31" t="s">
         <v>19</v>
@@ -2554,7 +2386,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2595,7 +2427,7 @@
         <v>16</v>
       </c>
       <c r="N32">
-        <v>0.59799999999999998</v>
+        <v>0.598</v>
       </c>
       <c r="O32" t="s">
         <v>19</v>
@@ -2607,7 +2439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2660,7 +2492,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2701,7 +2533,7 @@
         <v>16</v>
       </c>
       <c r="N34">
-        <v>0.23200000000000001</v>
+        <v>0.232</v>
       </c>
       <c r="O34" t="s">
         <v>23</v>
@@ -2713,7 +2545,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2724,7 +2556,7 @@
         <v>16</v>
       </c>
       <c r="D35">
-        <v>0.65700000000000003</v>
+        <v>0.657</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -2739,7 +2571,7 @@
         <v>16</v>
       </c>
       <c r="I35">
-        <v>0.65700000000000003</v>
+        <v>0.657</v>
       </c>
       <c r="J35" t="s">
         <v>19</v>
@@ -2754,7 +2586,7 @@
         <v>16</v>
       </c>
       <c r="N35">
-        <v>0.48899999999999999</v>
+        <v>0.489</v>
       </c>
       <c r="O35" t="s">
         <v>20</v>
@@ -2766,7 +2598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2807,7 +2639,7 @@
         <v>16</v>
       </c>
       <c r="N36">
-        <v>0.33300000000000002</v>
+        <v>0.333</v>
       </c>
       <c r="O36" t="s">
         <v>20</v>
@@ -2819,7 +2651,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2830,7 +2662,7 @@
         <v>16</v>
       </c>
       <c r="D37">
-        <v>0.52300000000000002</v>
+        <v>0.523</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -2845,7 +2677,7 @@
         <v>16</v>
       </c>
       <c r="I37">
-        <v>0.52300000000000002</v>
+        <v>0.523</v>
       </c>
       <c r="J37" t="s">
         <v>19</v>
@@ -2860,7 +2692,7 @@
         <v>16</v>
       </c>
       <c r="N37">
-        <v>0.35399999999999998</v>
+        <v>0.354</v>
       </c>
       <c r="O37" t="s">
         <v>20</v>
@@ -2872,7 +2704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2883,7 +2715,7 @@
         <v>16</v>
       </c>
       <c r="D38">
-        <v>0.57599999999999996</v>
+        <v>0.576</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -2898,7 +2730,7 @@
         <v>16</v>
       </c>
       <c r="I38">
-        <v>0.57599999999999996</v>
+        <v>0.576</v>
       </c>
       <c r="J38" t="s">
         <v>19</v>
@@ -2913,7 +2745,7 @@
         <v>16</v>
       </c>
       <c r="N38">
-        <v>0.40400000000000003</v>
+        <v>0.404</v>
       </c>
       <c r="O38" t="s">
         <v>20</v>
@@ -2925,7 +2757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2936,7 +2768,7 @@
         <v>16</v>
       </c>
       <c r="D39">
-        <v>0.53200000000000003</v>
+        <v>0.532</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
@@ -2951,7 +2783,7 @@
         <v>16</v>
       </c>
       <c r="I39">
-        <v>0.53200000000000003</v>
+        <v>0.532</v>
       </c>
       <c r="J39" t="s">
         <v>19</v>
@@ -2966,7 +2798,7 @@
         <v>16</v>
       </c>
       <c r="N39">
-        <v>0.36199999999999999</v>
+        <v>0.362</v>
       </c>
       <c r="O39" t="s">
         <v>20</v>
@@ -2978,7 +2810,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3019,7 +2851,7 @@
         <v>17</v>
       </c>
       <c r="N40">
-        <v>0.78100000000000003</v>
+        <v>0.781</v>
       </c>
       <c r="O40" t="s">
         <v>19</v>
@@ -3031,7 +2863,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3042,7 +2874,7 @@
         <v>16</v>
       </c>
       <c r="D41">
-        <v>0.52300000000000002</v>
+        <v>0.523</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
@@ -3057,7 +2889,7 @@
         <v>16</v>
       </c>
       <c r="I41">
-        <v>0.52300000000000002</v>
+        <v>0.523</v>
       </c>
       <c r="J41" t="s">
         <v>19</v>
@@ -3072,7 +2904,7 @@
         <v>16</v>
       </c>
       <c r="N41">
-        <v>0.35399999999999998</v>
+        <v>0.354</v>
       </c>
       <c r="O41" t="s">
         <v>20</v>
@@ -3084,7 +2916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3095,7 +2927,7 @@
         <v>17</v>
       </c>
       <c r="D42">
-        <v>0.95599999999999996</v>
+        <v>0.956</v>
       </c>
       <c r="E42" t="s">
         <v>18</v>
@@ -3110,7 +2942,7 @@
         <v>17</v>
       </c>
       <c r="I42">
-        <v>0.95599999999999996</v>
+        <v>0.956</v>
       </c>
       <c r="J42" t="s">
         <v>18</v>
@@ -3125,7 +2957,7 @@
         <v>17</v>
       </c>
       <c r="N42">
-        <v>0.91600000000000004</v>
+        <v>0.916</v>
       </c>
       <c r="O42" t="s">
         <v>18</v>
@@ -3137,18 +2969,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
       </c>
       <c r="D43">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
@@ -3157,13 +2989,13 @@
         <v>21</v>
       </c>
       <c r="G43">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H43" t="s">
         <v>17</v>
       </c>
       <c r="I43">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J43" t="s">
         <v>19</v>
@@ -3172,13 +3004,13 @@
         <v>21</v>
       </c>
       <c r="L43">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M43" t="s">
         <v>17</v>
       </c>
       <c r="N43">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O43" t="s">
         <v>20</v>
@@ -3190,7 +3022,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3201,7 +3033,7 @@
         <v>17</v>
       </c>
       <c r="D44">
-        <v>0.71099999999999997</v>
+        <v>0.711</v>
       </c>
       <c r="E44" t="s">
         <v>19</v>
@@ -3216,7 +3048,7 @@
         <v>17</v>
       </c>
       <c r="I44">
-        <v>0.71099999999999997</v>
+        <v>0.711</v>
       </c>
       <c r="J44" t="s">
         <v>19</v>
@@ -3231,7 +3063,7 @@
         <v>17</v>
       </c>
       <c r="N44">
-        <v>0.55100000000000005</v>
+        <v>0.551</v>
       </c>
       <c r="O44" t="s">
         <v>19</v>
@@ -3243,18 +3075,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
       </c>
       <c r="D45">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
@@ -3263,13 +3095,13 @@
         <v>21</v>
       </c>
       <c r="G45">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H45" t="s">
         <v>17</v>
       </c>
       <c r="I45">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J45" t="s">
         <v>19</v>
@@ -3278,13 +3110,13 @@
         <v>21</v>
       </c>
       <c r="L45">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M45" t="s">
         <v>17</v>
       </c>
       <c r="N45">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O45" t="s">
         <v>20</v>
@@ -3296,18 +3128,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
       </c>
       <c r="D46">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
@@ -3316,13 +3148,13 @@
         <v>21</v>
       </c>
       <c r="G46">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
       </c>
       <c r="I46">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J46" t="s">
         <v>19</v>
@@ -3331,13 +3163,13 @@
         <v>21</v>
       </c>
       <c r="L46">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M46" t="s">
         <v>17</v>
       </c>
       <c r="N46">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O46" t="s">
         <v>20</v>
@@ -3349,7 +3181,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3360,7 +3192,7 @@
         <v>16</v>
       </c>
       <c r="D47">
-        <v>0.69699999999999995</v>
+        <v>0.697</v>
       </c>
       <c r="E47" t="s">
         <v>19</v>
@@ -3375,7 +3207,7 @@
         <v>16</v>
       </c>
       <c r="I47">
-        <v>0.69699999999999995</v>
+        <v>0.697</v>
       </c>
       <c r="J47" t="s">
         <v>19</v>
@@ -3390,7 +3222,7 @@
         <v>16</v>
       </c>
       <c r="N47">
-        <v>0.53500000000000003</v>
+        <v>0.535</v>
       </c>
       <c r="O47" t="s">
         <v>19</v>
@@ -3402,7 +3234,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3413,7 +3245,7 @@
         <v>16</v>
       </c>
       <c r="D48">
-        <v>0.83899999999999997</v>
+        <v>0.839</v>
       </c>
       <c r="E48" t="s">
         <v>18</v>
@@ -3428,7 +3260,7 @@
         <v>16</v>
       </c>
       <c r="I48">
-        <v>0.83899999999999997</v>
+        <v>0.839</v>
       </c>
       <c r="J48" t="s">
         <v>18</v>
@@ -3443,7 +3275,7 @@
         <v>16</v>
       </c>
       <c r="N48">
-        <v>0.72199999999999998</v>
+        <v>0.722</v>
       </c>
       <c r="O48" t="s">
         <v>19</v>
@@ -3455,7 +3287,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3466,7 +3298,7 @@
         <v>17</v>
       </c>
       <c r="D49">
-        <v>0.80300000000000005</v>
+        <v>0.803</v>
       </c>
       <c r="E49" t="s">
         <v>18</v>
@@ -3481,7 +3313,7 @@
         <v>17</v>
       </c>
       <c r="I49">
-        <v>0.80300000000000005</v>
+        <v>0.803</v>
       </c>
       <c r="J49" t="s">
         <v>18</v>
@@ -3496,7 +3328,7 @@
         <v>17</v>
       </c>
       <c r="N49">
-        <v>0.67100000000000004</v>
+        <v>0.671</v>
       </c>
       <c r="O49" t="s">
         <v>19</v>
@@ -3508,7 +3340,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3519,7 +3351,7 @@
         <v>16</v>
       </c>
       <c r="D50">
-        <v>0.42599999999999999</v>
+        <v>0.426</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
@@ -3534,7 +3366,7 @@
         <v>16</v>
       </c>
       <c r="I50">
-        <v>0.42599999999999999</v>
+        <v>0.426</v>
       </c>
       <c r="J50" t="s">
         <v>20</v>
@@ -3549,7 +3381,7 @@
         <v>16</v>
       </c>
       <c r="N50">
-        <v>0.27100000000000002</v>
+        <v>0.271</v>
       </c>
       <c r="O50" t="s">
         <v>20</v>
@@ -3561,7 +3393,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3572,7 +3404,7 @@
         <v>16</v>
       </c>
       <c r="D51">
-        <v>0.54800000000000004</v>
+        <v>0.548</v>
       </c>
       <c r="E51" t="s">
         <v>19</v>
@@ -3587,7 +3419,7 @@
         <v>16</v>
       </c>
       <c r="I51">
-        <v>0.54800000000000004</v>
+        <v>0.548</v>
       </c>
       <c r="J51" t="s">
         <v>19</v>
@@ -3614,7 +3446,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3625,7 +3457,7 @@
         <v>17</v>
       </c>
       <c r="D52">
-        <v>0.51500000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="E52" t="s">
         <v>19</v>
@@ -3640,7 +3472,7 @@
         <v>17</v>
       </c>
       <c r="I52">
-        <v>0.51500000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="J52" t="s">
         <v>19</v>
@@ -3655,7 +3487,7 @@
         <v>17</v>
       </c>
       <c r="N52">
-        <v>0.34699999999999998</v>
+        <v>0.347</v>
       </c>
       <c r="O52" t="s">
         <v>20</v>
@@ -3667,7 +3499,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3708,7 +3540,7 @@
         <v>16</v>
       </c>
       <c r="N53">
-        <v>0.45700000000000002</v>
+        <v>0.457</v>
       </c>
       <c r="O53" t="s">
         <v>20</v>
@@ -3720,7 +3552,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3731,7 +3563,7 @@
         <v>16</v>
       </c>
       <c r="D54">
-        <v>0.75900000000000001</v>
+        <v>0.759</v>
       </c>
       <c r="E54" t="s">
         <v>19</v>
@@ -3746,7 +3578,7 @@
         <v>16</v>
       </c>
       <c r="I54">
-        <v>0.75900000000000001</v>
+        <v>0.759</v>
       </c>
       <c r="J54" t="s">
         <v>19</v>
@@ -3761,7 +3593,7 @@
         <v>16</v>
       </c>
       <c r="N54">
-        <v>0.61099999999999999</v>
+        <v>0.611</v>
       </c>
       <c r="O54" t="s">
         <v>19</v>
@@ -3773,7 +3605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3784,7 +3616,7 @@
         <v>16</v>
       </c>
       <c r="D55">
-        <v>0.89600000000000002</v>
+        <v>0.896</v>
       </c>
       <c r="E55" t="s">
         <v>18</v>
@@ -3799,7 +3631,7 @@
         <v>16</v>
       </c>
       <c r="I55">
-        <v>0.89600000000000002</v>
+        <v>0.896</v>
       </c>
       <c r="J55" t="s">
         <v>18</v>
@@ -3814,7 +3646,7 @@
         <v>16</v>
       </c>
       <c r="N55">
-        <v>0.81200000000000006</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="O55" t="s">
         <v>18</v>
@@ -3826,7 +3658,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3837,7 +3669,7 @@
         <v>16</v>
       </c>
       <c r="D56">
-        <v>0.59299999999999997</v>
+        <v>0.593</v>
       </c>
       <c r="E56" t="s">
         <v>19</v>
@@ -3852,7 +3684,7 @@
         <v>16</v>
       </c>
       <c r="I56">
-        <v>0.59299999999999997</v>
+        <v>0.593</v>
       </c>
       <c r="J56" t="s">
         <v>19</v>
@@ -3867,7 +3699,7 @@
         <v>16</v>
       </c>
       <c r="N56">
-        <v>0.42099999999999999</v>
+        <v>0.421</v>
       </c>
       <c r="O56" t="s">
         <v>20</v>
@@ -3879,7 +3711,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3890,7 +3722,7 @@
         <v>16</v>
       </c>
       <c r="D57">
-        <v>0.42599999999999999</v>
+        <v>0.426</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
@@ -3905,7 +3737,7 @@
         <v>16</v>
       </c>
       <c r="I57">
-        <v>0.42599999999999999</v>
+        <v>0.426</v>
       </c>
       <c r="J57" t="s">
         <v>20</v>
@@ -3920,7 +3752,7 @@
         <v>16</v>
       </c>
       <c r="N57">
-        <v>0.27100000000000002</v>
+        <v>0.271</v>
       </c>
       <c r="O57" t="s">
         <v>20</v>
@@ -3932,7 +3764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3973,7 +3805,7 @@
         <v>16</v>
       </c>
       <c r="N58">
-        <v>0.51500000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="O58" t="s">
         <v>19</v>
@@ -3985,7 +3817,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3996,7 +3828,7 @@
         <v>16</v>
       </c>
       <c r="D59">
-        <v>0.66300000000000003</v>
+        <v>0.663</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
@@ -4011,7 +3843,7 @@
         <v>16</v>
       </c>
       <c r="I59">
-        <v>0.66300000000000003</v>
+        <v>0.663</v>
       </c>
       <c r="J59" t="s">
         <v>19</v>
@@ -4038,7 +3870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4049,7 +3881,7 @@
         <v>17</v>
       </c>
       <c r="D60">
-        <v>0.95299999999999996</v>
+        <v>0.953</v>
       </c>
       <c r="E60" t="s">
         <v>18</v>
@@ -4064,7 +3896,7 @@
         <v>17</v>
       </c>
       <c r="I60">
-        <v>0.95299999999999996</v>
+        <v>0.953</v>
       </c>
       <c r="J60" t="s">
         <v>18</v>
@@ -4079,7 +3911,7 @@
         <v>17</v>
       </c>
       <c r="N60">
-        <v>0.90900000000000003</v>
+        <v>0.909</v>
       </c>
       <c r="O60" t="s">
         <v>18</v>
@@ -4091,7 +3923,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4102,7 +3934,7 @@
         <v>16</v>
       </c>
       <c r="D61">
-        <v>0.89800000000000002</v>
+        <v>0.898</v>
       </c>
       <c r="E61" t="s">
         <v>18</v>
@@ -4117,7 +3949,7 @@
         <v>16</v>
       </c>
       <c r="I61">
-        <v>0.89800000000000002</v>
+        <v>0.898</v>
       </c>
       <c r="J61" t="s">
         <v>18</v>
@@ -4132,7 +3964,7 @@
         <v>16</v>
       </c>
       <c r="N61">
-        <v>0.81499999999999995</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="O61" t="s">
         <v>18</v>
@@ -4144,7 +3976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4155,7 +3987,7 @@
         <v>16</v>
       </c>
       <c r="D62">
-        <v>0.85299999999999998</v>
+        <v>0.853</v>
       </c>
       <c r="E62" t="s">
         <v>18</v>
@@ -4170,7 +4002,7 @@
         <v>16</v>
       </c>
       <c r="I62">
-        <v>0.85299999999999998</v>
+        <v>0.853</v>
       </c>
       <c r="J62" t="s">
         <v>18</v>
@@ -4185,7 +4017,7 @@
         <v>16</v>
       </c>
       <c r="N62">
-        <v>0.74299999999999999</v>
+        <v>0.743</v>
       </c>
       <c r="O62" t="s">
         <v>19</v>
@@ -4197,7 +4029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4208,7 +4040,7 @@
         <v>16</v>
       </c>
       <c r="D63">
-        <v>0.69499999999999995</v>
+        <v>0.695</v>
       </c>
       <c r="E63" t="s">
         <v>19</v>
@@ -4223,7 +4055,7 @@
         <v>16</v>
       </c>
       <c r="I63">
-        <v>0.69499999999999995</v>
+        <v>0.695</v>
       </c>
       <c r="J63" t="s">
         <v>19</v>
@@ -4238,7 +4070,7 @@
         <v>16</v>
       </c>
       <c r="N63">
-        <v>0.53200000000000003</v>
+        <v>0.532</v>
       </c>
       <c r="O63" t="s">
         <v>19</v>
@@ -4250,7 +4082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4261,7 +4093,7 @@
         <v>16</v>
       </c>
       <c r="D64">
-        <v>0.76800000000000002</v>
+        <v>0.768</v>
       </c>
       <c r="E64" t="s">
         <v>19</v>
@@ -4276,7 +4108,7 @@
         <v>16</v>
       </c>
       <c r="I64">
-        <v>0.76800000000000002</v>
+        <v>0.768</v>
       </c>
       <c r="J64" t="s">
         <v>19</v>
@@ -4303,7 +4135,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4314,7 +4146,7 @@
         <v>17</v>
       </c>
       <c r="D65">
-        <v>0.91500000000000004</v>
+        <v>0.915</v>
       </c>
       <c r="E65" t="s">
         <v>18</v>
@@ -4329,7 +4161,7 @@
         <v>17</v>
       </c>
       <c r="I65">
-        <v>0.91500000000000004</v>
+        <v>0.915</v>
       </c>
       <c r="J65" t="s">
         <v>18</v>
@@ -4344,7 +4176,7 @@
         <v>17</v>
       </c>
       <c r="N65">
-        <v>0.84399999999999997</v>
+        <v>0.844</v>
       </c>
       <c r="O65" t="s">
         <v>18</v>
@@ -4356,12 +4188,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -4409,7 +4241,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4420,7 +4252,7 @@
         <v>16</v>
       </c>
       <c r="D67">
-        <v>0.82899999999999996</v>
+        <v>0.829</v>
       </c>
       <c r="E67" t="s">
         <v>18</v>
@@ -4435,7 +4267,7 @@
         <v>16</v>
       </c>
       <c r="I67">
-        <v>0.82899999999999996</v>
+        <v>0.829</v>
       </c>
       <c r="J67" t="s">
         <v>18</v>
@@ -4450,7 +4282,7 @@
         <v>16</v>
       </c>
       <c r="N67">
-        <v>0.70799999999999996</v>
+        <v>0.708</v>
       </c>
       <c r="O67" t="s">
         <v>19</v>
@@ -4462,7 +4294,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4473,7 +4305,7 @@
         <v>16</v>
       </c>
       <c r="D68">
-        <v>0.86899999999999999</v>
+        <v>0.869</v>
       </c>
       <c r="E68" t="s">
         <v>18</v>
@@ -4488,7 +4320,7 @@
         <v>16</v>
       </c>
       <c r="I68">
-        <v>0.86899999999999999</v>
+        <v>0.869</v>
       </c>
       <c r="J68" t="s">
         <v>18</v>
@@ -4503,7 +4335,7 @@
         <v>16</v>
       </c>
       <c r="N68">
-        <v>0.76900000000000002</v>
+        <v>0.769</v>
       </c>
       <c r="O68" t="s">
         <v>19</v>
@@ -4515,7 +4347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4526,7 +4358,7 @@
         <v>16</v>
       </c>
       <c r="D69">
-        <v>0.80500000000000005</v>
+        <v>0.805</v>
       </c>
       <c r="E69" t="s">
         <v>18</v>
@@ -4541,7 +4373,7 @@
         <v>16</v>
       </c>
       <c r="I69">
-        <v>0.80500000000000005</v>
+        <v>0.805</v>
       </c>
       <c r="J69" t="s">
         <v>18</v>
@@ -4556,7 +4388,7 @@
         <v>16</v>
       </c>
       <c r="N69">
-        <v>0.67300000000000004</v>
+        <v>0.673</v>
       </c>
       <c r="O69" t="s">
         <v>19</v>
@@ -4568,7 +4400,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4579,7 +4411,7 @@
         <v>16</v>
       </c>
       <c r="D70">
-        <v>0.53600000000000003</v>
+        <v>0.536</v>
       </c>
       <c r="E70" t="s">
         <v>19</v>
@@ -4594,7 +4426,7 @@
         <v>16</v>
       </c>
       <c r="I70">
-        <v>0.53600000000000003</v>
+        <v>0.536</v>
       </c>
       <c r="J70" t="s">
         <v>19</v>
@@ -4609,7 +4441,7 @@
         <v>16</v>
       </c>
       <c r="N70">
-        <v>0.36599999999999999</v>
+        <v>0.366</v>
       </c>
       <c r="O70" t="s">
         <v>20</v>
@@ -4621,7 +4453,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4632,7 +4464,7 @@
         <v>16</v>
       </c>
       <c r="D71">
-        <v>0.71799999999999997</v>
+        <v>0.718</v>
       </c>
       <c r="E71" t="s">
         <v>19</v>
@@ -4647,7 +4479,7 @@
         <v>16</v>
       </c>
       <c r="I71">
-        <v>0.71799999999999997</v>
+        <v>0.718</v>
       </c>
       <c r="J71" t="s">
         <v>19</v>
@@ -4662,7 +4494,7 @@
         <v>16</v>
       </c>
       <c r="N71">
-        <v>0.56000000000000005</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="O71" t="s">
         <v>19</v>
@@ -4674,7 +4506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4685,7 +4517,7 @@
         <v>17</v>
       </c>
       <c r="D72">
-        <v>0.71899999999999997</v>
+        <v>0.719</v>
       </c>
       <c r="E72" t="s">
         <v>19</v>
@@ -4700,7 +4532,7 @@
         <v>17</v>
       </c>
       <c r="I72">
-        <v>0.71899999999999997</v>
+        <v>0.719</v>
       </c>
       <c r="J72" t="s">
         <v>19</v>
@@ -4715,7 +4547,7 @@
         <v>17</v>
       </c>
       <c r="N72">
-        <v>0.56100000000000005</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="O72" t="s">
         <v>19</v>
@@ -4727,7 +4559,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4738,7 +4570,7 @@
         <v>17</v>
       </c>
       <c r="D73">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="E73" t="s">
         <v>18</v>
@@ -4753,7 +4585,7 @@
         <v>17</v>
       </c>
       <c r="I73">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="J73" t="s">
         <v>18</v>
@@ -4768,7 +4600,7 @@
         <v>17</v>
       </c>
       <c r="N73">
-        <v>0.73399999999999999</v>
+        <v>0.734</v>
       </c>
       <c r="O73" t="s">
         <v>19</v>
@@ -4780,7 +4612,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4833,7 +4665,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4886,7 +4718,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4939,18 +4771,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
         <v>17</v>
       </c>
       <c r="D77">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="E77" t="s">
         <v>18</v>
@@ -4959,13 +4791,13 @@
         <v>21</v>
       </c>
       <c r="G77">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H77" t="s">
         <v>17</v>
       </c>
       <c r="I77">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="J77" t="s">
         <v>18</v>
@@ -4974,13 +4806,13 @@
         <v>21</v>
       </c>
       <c r="L77">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M77" t="s">
         <v>17</v>
       </c>
       <c r="N77">
-        <v>0.73399999999999999</v>
+        <v>0.734</v>
       </c>
       <c r="O77" t="s">
         <v>19</v>
@@ -4992,12 +4824,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
         <v>17</v>
@@ -5045,12 +4877,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C79" t="s">
         <v>17</v>
@@ -5098,7 +4930,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5151,12 +4983,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C81" t="s">
         <v>17</v>
@@ -5204,7 +5036,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5215,7 +5047,7 @@
         <v>16</v>
       </c>
       <c r="D82">
-        <v>0.78100000000000003</v>
+        <v>0.781</v>
       </c>
       <c r="E82" t="s">
         <v>19</v>
@@ -5230,7 +5062,7 @@
         <v>16</v>
       </c>
       <c r="I82">
-        <v>0.78100000000000003</v>
+        <v>0.781</v>
       </c>
       <c r="J82" t="s">
         <v>19</v>
@@ -5257,7 +5089,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5268,7 +5100,7 @@
         <v>17</v>
       </c>
       <c r="D83">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="E83" t="s">
         <v>18</v>
@@ -5283,7 +5115,7 @@
         <v>17</v>
       </c>
       <c r="I83">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="J83" t="s">
         <v>18</v>
@@ -5298,7 +5130,7 @@
         <v>17</v>
       </c>
       <c r="N83">
-        <v>0.73399999999999999</v>
+        <v>0.734</v>
       </c>
       <c r="O83" t="s">
         <v>19</v>
@@ -5310,7 +5142,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5351,7 +5183,7 @@
         <v>16</v>
       </c>
       <c r="N84">
-        <v>0.72399999999999998</v>
+        <v>0.724</v>
       </c>
       <c r="O84" t="s">
         <v>19</v>
@@ -5363,18 +5195,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s">
         <v>17</v>
       </c>
       <c r="D85">
-        <v>0.70899999999999996</v>
+        <v>0.709</v>
       </c>
       <c r="E85" t="s">
         <v>19</v>
@@ -5389,7 +5221,7 @@
         <v>17</v>
       </c>
       <c r="I85">
-        <v>0.70899999999999996</v>
+        <v>0.709</v>
       </c>
       <c r="J85" t="s">
         <v>19</v>
@@ -5398,13 +5230,13 @@
         <v>21</v>
       </c>
       <c r="L85">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M85" t="s">
         <v>17</v>
       </c>
       <c r="N85">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="O85" t="s">
         <v>19</v>
@@ -5416,7 +5248,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5457,7 +5289,7 @@
         <v>16</v>
       </c>
       <c r="N86">
-        <v>0.28199999999999997</v>
+        <v>0.282</v>
       </c>
       <c r="O86" t="s">
         <v>20</v>
@@ -5469,7 +5301,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5480,7 +5312,7 @@
         <v>17</v>
       </c>
       <c r="D87">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="E87" t="s">
         <v>18</v>
@@ -5495,7 +5327,7 @@
         <v>17</v>
       </c>
       <c r="I87">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="J87" t="s">
         <v>18</v>
@@ -5510,7 +5342,7 @@
         <v>17</v>
       </c>
       <c r="N87">
-        <v>0.73399999999999999</v>
+        <v>0.734</v>
       </c>
       <c r="O87" t="s">
         <v>19</v>
@@ -5522,18 +5354,18 @@
         <v>108</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s">
         <v>16</v>
       </c>
       <c r="D88">
-        <v>0.80100000000000005</v>
+        <v>0.801</v>
       </c>
       <c r="E88" t="s">
         <v>18</v>
@@ -5542,13 +5374,13 @@
         <v>21</v>
       </c>
       <c r="G88">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H88" t="s">
         <v>16</v>
       </c>
       <c r="I88">
-        <v>0.80100000000000005</v>
+        <v>0.801</v>
       </c>
       <c r="J88" t="s">
         <v>18</v>
@@ -5557,13 +5389,13 @@
         <v>21</v>
       </c>
       <c r="L88">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M88" t="s">
         <v>16</v>
       </c>
       <c r="N88">
-        <v>0.66800000000000004</v>
+        <v>0.668</v>
       </c>
       <c r="O88" t="s">
         <v>19</v>
@@ -5575,7 +5407,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5586,7 +5418,7 @@
         <v>17</v>
       </c>
       <c r="D89">
-        <v>0.96099999999999997</v>
+        <v>0.961</v>
       </c>
       <c r="E89" t="s">
         <v>18</v>
@@ -5601,7 +5433,7 @@
         <v>17</v>
       </c>
       <c r="I89">
-        <v>0.96099999999999997</v>
+        <v>0.961</v>
       </c>
       <c r="J89" t="s">
         <v>18</v>
@@ -5616,7 +5448,7 @@
         <v>17</v>
       </c>
       <c r="N89">
-        <v>0.92500000000000004</v>
+        <v>0.925</v>
       </c>
       <c r="O89" t="s">
         <v>18</v>
@@ -5628,7 +5460,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5639,7 +5471,7 @@
         <v>16</v>
       </c>
       <c r="D90">
-        <v>0.73899999999999999</v>
+        <v>0.739</v>
       </c>
       <c r="E90" t="s">
         <v>19</v>
@@ -5654,7 +5486,7 @@
         <v>16</v>
       </c>
       <c r="I90">
-        <v>0.73899999999999999</v>
+        <v>0.739</v>
       </c>
       <c r="J90" t="s">
         <v>19</v>
@@ -5669,7 +5501,7 @@
         <v>16</v>
       </c>
       <c r="N90">
-        <v>0.58499999999999996</v>
+        <v>0.585</v>
       </c>
       <c r="O90" t="s">
         <v>19</v>
@@ -5681,7 +5513,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5692,7 +5524,7 @@
         <v>16</v>
       </c>
       <c r="D91">
-        <v>0.59599999999999997</v>
+        <v>0.596</v>
       </c>
       <c r="E91" t="s">
         <v>19</v>
@@ -5707,7 +5539,7 @@
         <v>16</v>
       </c>
       <c r="I91">
-        <v>0.59599999999999997</v>
+        <v>0.596</v>
       </c>
       <c r="J91" t="s">
         <v>19</v>
@@ -5722,7 +5554,7 @@
         <v>16</v>
       </c>
       <c r="N91">
-        <v>0.42399999999999999</v>
+        <v>0.424</v>
       </c>
       <c r="O91" t="s">
         <v>20</v>
@@ -5734,7 +5566,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5745,7 +5577,7 @@
         <v>16</v>
       </c>
       <c r="D92">
-        <v>0.51300000000000001</v>
+        <v>0.513</v>
       </c>
       <c r="E92" t="s">
         <v>19</v>
@@ -5760,7 +5592,7 @@
         <v>16</v>
       </c>
       <c r="I92">
-        <v>0.51300000000000001</v>
+        <v>0.513</v>
       </c>
       <c r="J92" t="s">
         <v>19</v>
@@ -5775,7 +5607,7 @@
         <v>16</v>
       </c>
       <c r="N92">
-        <v>0.34499999999999997</v>
+        <v>0.345</v>
       </c>
       <c r="O92" t="s">
         <v>20</v>
@@ -5787,7 +5619,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5798,7 +5630,7 @@
         <v>16</v>
       </c>
       <c r="D93">
-        <v>0.76300000000000001</v>
+        <v>0.763</v>
       </c>
       <c r="E93" t="s">
         <v>19</v>
@@ -5813,7 +5645,7 @@
         <v>16</v>
       </c>
       <c r="I93">
-        <v>0.76300000000000001</v>
+        <v>0.763</v>
       </c>
       <c r="J93" t="s">
         <v>19</v>
@@ -5828,7 +5660,7 @@
         <v>16</v>
       </c>
       <c r="N93">
-        <v>0.61699999999999999</v>
+        <v>0.617</v>
       </c>
       <c r="O93" t="s">
         <v>19</v>
@@ -5840,7 +5672,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5851,7 +5683,7 @@
         <v>16</v>
       </c>
       <c r="D94">
-        <v>0.89300000000000002</v>
+        <v>0.893</v>
       </c>
       <c r="E94" t="s">
         <v>18</v>
@@ -5866,7 +5698,7 @@
         <v>16</v>
       </c>
       <c r="I94">
-        <v>0.89300000000000002</v>
+        <v>0.893</v>
       </c>
       <c r="J94" t="s">
         <v>18</v>
@@ -5881,7 +5713,7 @@
         <v>16</v>
       </c>
       <c r="N94">
-        <v>0.80700000000000005</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="O94" t="s">
         <v>18</v>
@@ -5893,7 +5725,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5946,7 +5778,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5999,18 +5831,18 @@
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C97" t="s">
         <v>17</v>
       </c>
       <c r="D97">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="E97" t="s">
         <v>18</v>
@@ -6019,13 +5851,13 @@
         <v>21</v>
       </c>
       <c r="G97">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H97" t="s">
         <v>17</v>
       </c>
       <c r="I97">
-        <v>0.84699999999999998</v>
+        <v>0.847</v>
       </c>
       <c r="J97" t="s">
         <v>18</v>
@@ -6034,13 +5866,13 @@
         <v>21</v>
       </c>
       <c r="L97">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M97" t="s">
         <v>17</v>
       </c>
       <c r="N97">
-        <v>0.73399999999999999</v>
+        <v>0.734</v>
       </c>
       <c r="O97" t="s">
         <v>19</v>
@@ -6052,7 +5884,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6063,7 +5895,7 @@
         <v>16</v>
       </c>
       <c r="D98">
-        <v>0.46200000000000002</v>
+        <v>0.462</v>
       </c>
       <c r="E98" t="s">
         <v>20</v>
@@ -6078,7 +5910,7 @@
         <v>16</v>
       </c>
       <c r="I98">
-        <v>0.46200000000000002</v>
+        <v>0.462</v>
       </c>
       <c r="J98" t="s">
         <v>20</v>
@@ -6105,7 +5937,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6116,7 +5948,7 @@
         <v>16</v>
       </c>
       <c r="D99">
-        <v>0.69699999999999995</v>
+        <v>0.697</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
@@ -6131,7 +5963,7 @@
         <v>16</v>
       </c>
       <c r="I99">
-        <v>0.69699999999999995</v>
+        <v>0.697</v>
       </c>
       <c r="J99" t="s">
         <v>19</v>
@@ -6146,7 +5978,7 @@
         <v>16</v>
       </c>
       <c r="N99">
-        <v>0.53600000000000003</v>
+        <v>0.536</v>
       </c>
       <c r="O99" t="s">
         <v>19</v>
@@ -6158,12 +5990,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
         <v>17</v>
@@ -6178,7 +6010,7 @@
         <v>21</v>
       </c>
       <c r="G100">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H100" t="s">
         <v>17</v>
@@ -6193,7 +6025,7 @@
         <v>21</v>
       </c>
       <c r="L100">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M100" t="s">
         <v>17</v>
@@ -6211,7 +6043,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6222,7 +6054,7 @@
         <v>17</v>
       </c>
       <c r="D101">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="E101" t="s">
         <v>19</v>
@@ -6237,7 +6069,7 @@
         <v>17</v>
       </c>
       <c r="I101">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="J101" t="s">
         <v>19</v>
@@ -6252,7 +6084,7 @@
         <v>17</v>
       </c>
       <c r="N101">
-        <v>0.40799999999999997</v>
+        <v>0.408</v>
       </c>
       <c r="O101" t="s">
         <v>20</v>
@@ -6266,8 +6098,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>